<commit_message>
added 2 new entries to survey dataset
</commit_message>
<xml_diff>
--- a/TurkeySurveyDataFlippedWithCategories.xlsx
+++ b/TurkeySurveyDataFlippedWithCategories.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\emily\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\emily\GitHub\Final_Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6C222AA-D3A3-412B-8CFC-8319B7502961}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BFC89A5-94E0-47D1-A445-F6322E9502C3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-4815" windowWidth="29040" windowHeight="16440" xr2:uid="{734DAC25-DDEB-4002-9D76-72D64F7C83B2}"/>
   </bookViews>
@@ -30,6 +30,24 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>tc={11B96AB9-66A1-4AEA-8C31-44BA6E9027DF}</author>
+  </authors>
+  <commentList>
+    <comment ref="FP1" authorId="0" shapeId="0" xr:uid="{11B96AB9-66A1-4AEA-8C31-44BA6E9027DF}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    new USA entries start at 171</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
@@ -234,7 +252,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -251,13 +269,37 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -272,9 +314,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -290,6 +334,12 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <person displayName="emily.j.boling@outlook.com" id="{291B16D1-E622-4C05-8DBC-3EE79E13938A}" userId="503711c3c454736e" providerId="Windows Live"/>
+</personList>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -587,1058 +637,1081 @@
 </a:theme>
 </file>
 
+<file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="FP1" dT="2020-03-14T21:22:00.80" personId="{291B16D1-E622-4C05-8DBC-3EE79E13938A}" id="{11B96AB9-66A1-4AEA-8C31-44BA6E9027DF}">
+    <text>new USA entries start at 171</text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39A11758-560F-4C1B-85CE-C181E38F2ED2}">
-  <dimension ref="A1:FQ56"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39A11758-560F-4C1B-85CE-C181E38F2ED2}">
+  <dimension ref="A1:FV56"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="FQ3" sqref="FQ3:FQ56"/>
+    <sheetView tabSelected="1" topLeftCell="EU1" workbookViewId="0">
+      <selection activeCell="FR14" sqref="FR14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="172" max="172" width="27" bestFit="1" customWidth="1"/>
-    <col min="173" max="173" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="177" max="177" width="27" bestFit="1" customWidth="1"/>
+    <col min="178" max="178" width="17.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:173" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:178" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1">
-        <v>1</v>
-      </c>
-      <c r="C1">
-        <v>2</v>
-      </c>
-      <c r="D1">
-        <v>3</v>
-      </c>
-      <c r="E1">
-        <v>4</v>
-      </c>
-      <c r="F1">
+      <c r="B1" s="1">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1">
         <v>5</v>
       </c>
-      <c r="G1">
+      <c r="G1" s="1">
         <v>6</v>
       </c>
-      <c r="H1">
+      <c r="H1" s="1">
         <v>7</v>
       </c>
-      <c r="I1">
+      <c r="I1" s="1">
         <v>8</v>
       </c>
-      <c r="J1">
+      <c r="J1" s="1">
         <v>9</v>
       </c>
-      <c r="K1">
+      <c r="K1" s="1">
         <v>10</v>
       </c>
-      <c r="L1">
+      <c r="L1" s="1">
         <v>11</v>
       </c>
-      <c r="M1">
+      <c r="M1" s="1">
         <v>12</v>
       </c>
-      <c r="N1">
+      <c r="N1" s="1">
         <v>13</v>
       </c>
-      <c r="O1">
+      <c r="O1" s="1">
         <v>14</v>
       </c>
-      <c r="P1">
+      <c r="P1" s="1">
         <v>15</v>
       </c>
-      <c r="Q1">
+      <c r="Q1" s="1">
         <v>16</v>
       </c>
-      <c r="R1">
+      <c r="R1" s="1">
         <v>17</v>
       </c>
-      <c r="S1">
+      <c r="S1" s="1">
         <v>18</v>
       </c>
-      <c r="T1">
+      <c r="T1" s="1">
         <v>19</v>
       </c>
-      <c r="U1">
+      <c r="U1" s="1">
         <v>20</v>
       </c>
-      <c r="V1">
+      <c r="V1" s="1">
         <v>21</v>
       </c>
-      <c r="W1">
+      <c r="W1" s="1">
         <v>22</v>
       </c>
-      <c r="X1">
+      <c r="X1" s="1">
         <v>23</v>
       </c>
-      <c r="Y1">
+      <c r="Y1" s="1">
         <v>24</v>
       </c>
-      <c r="Z1">
+      <c r="Z1" s="1">
         <v>25</v>
       </c>
-      <c r="AA1">
+      <c r="AA1" s="1">
         <v>26</v>
       </c>
-      <c r="AB1">
+      <c r="AB1" s="1">
         <v>27</v>
       </c>
-      <c r="AC1">
+      <c r="AC1" s="1">
         <v>28</v>
       </c>
-      <c r="AD1">
+      <c r="AD1" s="1">
         <v>29</v>
       </c>
-      <c r="AE1">
+      <c r="AE1" s="1">
         <v>30</v>
       </c>
-      <c r="AF1">
+      <c r="AF1" s="1">
         <v>31</v>
       </c>
-      <c r="AG1">
+      <c r="AG1" s="1">
         <v>32</v>
       </c>
-      <c r="AH1">
+      <c r="AH1" s="1">
         <v>33</v>
       </c>
-      <c r="AI1">
+      <c r="AI1" s="1">
         <v>34</v>
       </c>
-      <c r="AJ1">
+      <c r="AJ1" s="1">
         <v>35</v>
       </c>
-      <c r="AK1">
+      <c r="AK1" s="1">
         <v>36</v>
       </c>
-      <c r="AL1">
+      <c r="AL1" s="1">
         <v>37</v>
       </c>
-      <c r="AM1">
+      <c r="AM1" s="1">
         <v>38</v>
       </c>
-      <c r="AN1">
+      <c r="AN1" s="1">
         <v>39</v>
       </c>
-      <c r="AO1">
+      <c r="AO1" s="1">
         <v>40</v>
       </c>
-      <c r="AP1">
+      <c r="AP1" s="1">
         <v>41</v>
       </c>
-      <c r="AQ1">
+      <c r="AQ1" s="1">
         <v>42</v>
       </c>
-      <c r="AR1">
+      <c r="AR1" s="1">
         <v>43</v>
       </c>
-      <c r="AS1">
+      <c r="AS1" s="1">
         <v>44</v>
       </c>
-      <c r="AT1">
+      <c r="AT1" s="1">
         <v>45</v>
       </c>
-      <c r="AU1">
+      <c r="AU1" s="1">
         <v>46</v>
       </c>
-      <c r="AV1">
+      <c r="AV1" s="1">
         <v>47</v>
       </c>
-      <c r="AW1">
+      <c r="AW1" s="1">
         <v>48</v>
       </c>
-      <c r="AX1">
+      <c r="AX1" s="1">
         <v>49</v>
       </c>
-      <c r="AY1">
+      <c r="AY1" s="1">
         <v>50</v>
       </c>
-      <c r="AZ1">
+      <c r="AZ1" s="1">
         <v>51</v>
       </c>
-      <c r="BA1">
+      <c r="BA1" s="1">
         <v>52</v>
       </c>
-      <c r="BB1">
+      <c r="BB1" s="1">
         <v>53</v>
       </c>
-      <c r="BC1">
+      <c r="BC1" s="1">
         <v>54</v>
       </c>
-      <c r="BD1">
+      <c r="BD1" s="1">
         <v>55</v>
       </c>
-      <c r="BE1">
+      <c r="BE1" s="1">
         <v>56</v>
       </c>
-      <c r="BF1">
+      <c r="BF1" s="1">
         <v>57</v>
       </c>
-      <c r="BG1">
+      <c r="BG1" s="1">
         <v>58</v>
       </c>
-      <c r="BH1">
+      <c r="BH1" s="1">
         <v>59</v>
       </c>
-      <c r="BI1">
+      <c r="BI1" s="1">
         <v>60</v>
       </c>
-      <c r="BJ1">
+      <c r="BJ1" s="1">
         <v>61</v>
       </c>
-      <c r="BK1">
+      <c r="BK1" s="1">
         <v>62</v>
       </c>
-      <c r="BL1">
+      <c r="BL1" s="1">
         <v>63</v>
       </c>
-      <c r="BM1">
+      <c r="BM1" s="1">
         <v>64</v>
       </c>
-      <c r="BN1">
+      <c r="BN1" s="1">
         <v>65</v>
       </c>
-      <c r="BO1">
+      <c r="BO1" s="1">
         <v>66</v>
       </c>
-      <c r="BP1">
+      <c r="BP1" s="1">
         <v>67</v>
       </c>
-      <c r="BQ1">
+      <c r="BQ1" s="1">
         <v>68</v>
       </c>
-      <c r="BR1">
+      <c r="BR1" s="1">
         <v>69</v>
       </c>
-      <c r="BS1">
+      <c r="BS1" s="1">
         <v>70</v>
       </c>
-      <c r="BT1">
+      <c r="BT1" s="1">
         <v>71</v>
       </c>
-      <c r="BU1">
+      <c r="BU1" s="1">
         <v>72</v>
       </c>
-      <c r="BV1">
+      <c r="BV1" s="1">
         <v>73</v>
       </c>
-      <c r="BW1">
+      <c r="BW1" s="1">
         <v>74</v>
       </c>
-      <c r="BX1">
+      <c r="BX1" s="1">
         <v>75</v>
       </c>
-      <c r="BY1">
+      <c r="BY1" s="1">
         <v>76</v>
       </c>
-      <c r="BZ1">
+      <c r="BZ1" s="1">
         <v>77</v>
       </c>
-      <c r="CA1">
+      <c r="CA1" s="1">
         <v>78</v>
       </c>
-      <c r="CB1">
+      <c r="CB1" s="1">
         <v>79</v>
       </c>
-      <c r="CC1">
+      <c r="CC1" s="1">
         <v>80</v>
       </c>
-      <c r="CD1">
+      <c r="CD1" s="1">
         <v>81</v>
       </c>
-      <c r="CE1">
+      <c r="CE1" s="1">
         <v>82</v>
       </c>
-      <c r="CF1">
+      <c r="CF1" s="1">
         <v>83</v>
       </c>
-      <c r="CG1">
+      <c r="CG1" s="1">
         <v>84</v>
       </c>
-      <c r="CH1">
+      <c r="CH1" s="1">
         <v>85</v>
       </c>
-      <c r="CI1">
+      <c r="CI1" s="1">
         <v>86</v>
       </c>
-      <c r="CJ1">
+      <c r="CJ1" s="1">
         <v>87</v>
       </c>
-      <c r="CK1">
+      <c r="CK1" s="1">
         <v>88</v>
       </c>
-      <c r="CL1">
+      <c r="CL1" s="1">
         <v>89</v>
       </c>
-      <c r="CM1">
+      <c r="CM1" s="1">
         <v>90</v>
       </c>
-      <c r="CN1">
+      <c r="CN1" s="1">
         <v>91</v>
       </c>
-      <c r="CO1">
+      <c r="CO1" s="1">
         <v>92</v>
       </c>
-      <c r="CP1">
+      <c r="CP1" s="1">
         <v>93</v>
       </c>
-      <c r="CQ1">
+      <c r="CQ1" s="1">
         <v>94</v>
       </c>
-      <c r="CR1">
+      <c r="CR1" s="1">
         <v>95</v>
       </c>
-      <c r="CS1">
+      <c r="CS1" s="1">
         <v>96</v>
       </c>
-      <c r="CT1">
+      <c r="CT1" s="1">
         <v>97</v>
       </c>
-      <c r="CU1">
+      <c r="CU1" s="1">
         <v>98</v>
       </c>
-      <c r="CV1">
+      <c r="CV1" s="1">
         <v>99</v>
       </c>
-      <c r="CW1">
+      <c r="CW1" s="1">
         <v>100</v>
       </c>
-      <c r="CX1">
+      <c r="CX1" s="1">
         <v>101</v>
       </c>
-      <c r="CY1">
+      <c r="CY1" s="1">
         <v>102</v>
       </c>
-      <c r="CZ1">
+      <c r="CZ1" s="1">
         <v>103</v>
       </c>
-      <c r="DA1">
+      <c r="DA1" s="1">
         <v>104</v>
       </c>
-      <c r="DB1">
+      <c r="DB1" s="1">
         <v>105</v>
       </c>
-      <c r="DC1">
+      <c r="DC1" s="1">
         <v>106</v>
       </c>
-      <c r="DD1">
+      <c r="DD1" s="1">
         <v>107</v>
       </c>
-      <c r="DE1">
+      <c r="DE1" s="1">
         <v>108</v>
       </c>
-      <c r="DF1">
+      <c r="DF1" s="1">
         <v>109</v>
       </c>
-      <c r="DG1">
+      <c r="DG1" s="1">
         <v>110</v>
       </c>
-      <c r="DH1">
+      <c r="DH1" s="1">
         <v>111</v>
       </c>
-      <c r="DI1">
+      <c r="DI1" s="1">
         <v>112</v>
       </c>
-      <c r="DJ1">
+      <c r="DJ1" s="1">
         <v>113</v>
       </c>
-      <c r="DK1">
+      <c r="DK1" s="1">
         <v>114</v>
       </c>
-      <c r="DL1">
+      <c r="DL1" s="1">
         <v>115</v>
       </c>
-      <c r="DM1">
+      <c r="DM1" s="1">
         <v>116</v>
       </c>
-      <c r="DN1">
+      <c r="DN1" s="1">
         <v>117</v>
       </c>
-      <c r="DO1">
+      <c r="DO1" s="1">
         <v>118</v>
       </c>
-      <c r="DP1">
+      <c r="DP1" s="1">
         <v>119</v>
       </c>
-      <c r="DQ1">
+      <c r="DQ1" s="1">
         <v>120</v>
       </c>
-      <c r="DR1">
+      <c r="DR1" s="1">
         <v>121</v>
       </c>
-      <c r="DS1">
+      <c r="DS1" s="1">
         <v>122</v>
       </c>
-      <c r="DT1">
+      <c r="DT1" s="1">
         <v>123</v>
       </c>
-      <c r="DU1">
+      <c r="DU1" s="1">
         <v>124</v>
       </c>
-      <c r="DV1">
+      <c r="DV1" s="1">
         <v>125</v>
       </c>
-      <c r="DW1">
+      <c r="DW1" s="1">
         <v>126</v>
       </c>
-      <c r="DX1">
+      <c r="DX1" s="1">
         <v>127</v>
       </c>
-      <c r="DY1">
+      <c r="DY1" s="1">
         <v>128</v>
       </c>
-      <c r="DZ1">
+      <c r="DZ1" s="1">
         <v>129</v>
       </c>
-      <c r="EA1">
+      <c r="EA1" s="1">
         <v>130</v>
       </c>
-      <c r="EB1">
+      <c r="EB1" s="1">
         <v>131</v>
       </c>
-      <c r="EC1">
+      <c r="EC1" s="1">
         <v>132</v>
       </c>
-      <c r="ED1">
+      <c r="ED1" s="1">
         <v>133</v>
       </c>
-      <c r="EE1">
+      <c r="EE1" s="1">
         <v>134</v>
       </c>
-      <c r="EF1">
+      <c r="EF1" s="1">
         <v>135</v>
       </c>
-      <c r="EG1">
+      <c r="EG1" s="1">
         <v>136</v>
       </c>
-      <c r="EH1">
+      <c r="EH1" s="1">
         <v>137</v>
       </c>
-      <c r="EI1">
+      <c r="EI1" s="1">
         <v>138</v>
       </c>
-      <c r="EJ1">
+      <c r="EJ1" s="1">
         <v>139</v>
       </c>
-      <c r="EK1">
+      <c r="EK1" s="1">
         <v>140</v>
       </c>
-      <c r="EL1">
+      <c r="EL1" s="1">
         <v>141</v>
       </c>
-      <c r="EM1">
+      <c r="EM1" s="1">
         <v>142</v>
       </c>
-      <c r="EN1">
+      <c r="EN1" s="1">
         <v>143</v>
       </c>
-      <c r="EO1">
+      <c r="EO1" s="1">
         <v>144</v>
       </c>
-      <c r="EP1">
+      <c r="EP1" s="1">
         <v>145</v>
       </c>
-      <c r="EQ1">
+      <c r="EQ1" s="1">
         <v>146</v>
       </c>
-      <c r="ER1">
+      <c r="ER1" s="1">
         <v>147</v>
       </c>
-      <c r="ES1">
+      <c r="ES1" s="1">
         <v>148</v>
       </c>
-      <c r="ET1">
+      <c r="ET1" s="1">
         <v>149</v>
       </c>
-      <c r="EU1">
+      <c r="EU1" s="1">
         <v>150</v>
       </c>
-      <c r="EV1">
+      <c r="EV1" s="1">
         <v>151</v>
       </c>
-      <c r="EW1">
+      <c r="EW1" s="1">
         <v>152</v>
       </c>
-      <c r="EX1">
+      <c r="EX1" s="1">
         <v>153</v>
       </c>
-      <c r="EY1">
+      <c r="EY1" s="1">
         <v>154</v>
       </c>
-      <c r="EZ1">
+      <c r="EZ1" s="1">
         <v>155</v>
       </c>
-      <c r="FA1">
+      <c r="FA1" s="1">
         <v>156</v>
       </c>
-      <c r="FB1">
+      <c r="FB1" s="1">
         <v>157</v>
       </c>
-      <c r="FC1">
+      <c r="FC1" s="1">
         <v>158</v>
       </c>
-      <c r="FD1">
+      <c r="FD1" s="1">
         <v>159</v>
       </c>
-      <c r="FE1">
+      <c r="FE1" s="1">
         <v>160</v>
       </c>
-      <c r="FF1">
+      <c r="FF1" s="1">
         <v>161</v>
       </c>
-      <c r="FG1">
+      <c r="FG1" s="1">
         <v>162</v>
       </c>
-      <c r="FH1">
+      <c r="FH1" s="1">
         <v>163</v>
       </c>
-      <c r="FI1">
+      <c r="FI1" s="1">
         <v>164</v>
       </c>
-      <c r="FJ1">
+      <c r="FJ1" s="1">
         <v>165</v>
       </c>
-      <c r="FK1">
+      <c r="FK1" s="1">
         <v>166</v>
       </c>
-      <c r="FL1">
+      <c r="FL1" s="1">
         <v>167</v>
       </c>
-      <c r="FM1">
+      <c r="FM1" s="1">
         <v>168</v>
       </c>
-      <c r="FN1">
+      <c r="FN1" s="1">
         <v>169</v>
       </c>
-      <c r="FO1">
+      <c r="FO1" s="1">
         <v>170</v>
       </c>
-      <c r="FP1" t="s">
+      <c r="FP1" s="3">
+        <v>171</v>
+      </c>
+      <c r="FQ1" s="3">
+        <v>172</v>
+      </c>
+      <c r="FR1" s="3"/>
+      <c r="FS1" s="3"/>
+      <c r="FT1" s="3"/>
+      <c r="FU1" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="FQ1" t="s">
+      <c r="FV1" s="1" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="2" spans="1:173" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="1:178" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="B2">
-        <v>1</v>
-      </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
-      <c r="D2">
-        <v>1</v>
-      </c>
-      <c r="E2">
-        <v>1</v>
-      </c>
-      <c r="F2">
-        <v>1</v>
-      </c>
-      <c r="G2">
-        <v>1</v>
-      </c>
-      <c r="H2">
-        <v>1</v>
-      </c>
-      <c r="I2">
-        <v>1</v>
-      </c>
-      <c r="J2">
-        <v>1</v>
-      </c>
-      <c r="K2">
-        <v>1</v>
-      </c>
-      <c r="L2">
-        <v>1</v>
-      </c>
-      <c r="M2">
-        <v>1</v>
-      </c>
-      <c r="N2">
-        <v>1</v>
-      </c>
-      <c r="O2">
-        <v>1</v>
-      </c>
-      <c r="P2">
-        <v>1</v>
-      </c>
-      <c r="Q2">
-        <v>1</v>
-      </c>
-      <c r="R2">
-        <v>1</v>
-      </c>
-      <c r="S2">
-        <v>1</v>
-      </c>
-      <c r="T2">
-        <v>1</v>
-      </c>
-      <c r="U2">
-        <v>1</v>
-      </c>
-      <c r="V2">
-        <v>1</v>
-      </c>
-      <c r="W2">
-        <v>1</v>
-      </c>
-      <c r="X2">
-        <v>1</v>
-      </c>
-      <c r="Y2">
-        <v>1</v>
-      </c>
-      <c r="Z2">
-        <v>1</v>
-      </c>
-      <c r="AA2">
-        <v>1</v>
-      </c>
-      <c r="AB2">
-        <v>1</v>
-      </c>
-      <c r="AC2">
-        <v>1</v>
-      </c>
-      <c r="AD2">
-        <v>1</v>
-      </c>
-      <c r="AE2">
-        <v>1</v>
-      </c>
-      <c r="AF2">
-        <v>1</v>
-      </c>
-      <c r="AG2">
-        <v>1</v>
-      </c>
-      <c r="AH2">
-        <v>1</v>
-      </c>
-      <c r="AI2">
-        <v>1</v>
-      </c>
-      <c r="AJ2">
-        <v>1</v>
-      </c>
-      <c r="AK2">
-        <v>1</v>
-      </c>
-      <c r="AL2">
-        <v>1</v>
-      </c>
-      <c r="AM2">
-        <v>1</v>
-      </c>
-      <c r="AN2">
-        <v>1</v>
-      </c>
-      <c r="AO2">
-        <v>1</v>
-      </c>
-      <c r="AP2">
-        <v>1</v>
-      </c>
-      <c r="AQ2">
-        <v>1</v>
-      </c>
-      <c r="AR2">
-        <v>1</v>
-      </c>
-      <c r="AS2">
-        <v>1</v>
-      </c>
-      <c r="AT2">
-        <v>1</v>
-      </c>
-      <c r="AU2">
-        <v>1</v>
-      </c>
-      <c r="AV2">
-        <v>1</v>
-      </c>
-      <c r="AW2">
-        <v>1</v>
-      </c>
-      <c r="AX2">
-        <v>1</v>
-      </c>
-      <c r="AY2">
-        <v>1</v>
-      </c>
-      <c r="AZ2">
-        <v>1</v>
-      </c>
-      <c r="BA2">
-        <v>1</v>
-      </c>
-      <c r="BB2">
-        <v>1</v>
-      </c>
-      <c r="BC2">
-        <v>1</v>
-      </c>
-      <c r="BD2">
-        <v>1</v>
-      </c>
-      <c r="BE2">
-        <v>1</v>
-      </c>
-      <c r="BF2">
-        <v>1</v>
-      </c>
-      <c r="BG2">
-        <v>1</v>
-      </c>
-      <c r="BH2">
-        <v>1</v>
-      </c>
-      <c r="BI2">
-        <v>1</v>
-      </c>
-      <c r="BJ2">
-        <v>1</v>
-      </c>
-      <c r="BK2">
-        <v>1</v>
-      </c>
-      <c r="BL2">
-        <v>1</v>
-      </c>
-      <c r="BM2">
-        <v>1</v>
-      </c>
-      <c r="BN2">
-        <v>1</v>
-      </c>
-      <c r="BO2">
-        <v>1</v>
-      </c>
-      <c r="BP2">
-        <v>1</v>
-      </c>
-      <c r="BQ2">
-        <v>1</v>
-      </c>
-      <c r="BR2">
-        <v>1</v>
-      </c>
-      <c r="BS2">
-        <v>1</v>
-      </c>
-      <c r="BT2">
-        <v>1</v>
-      </c>
-      <c r="BU2">
-        <v>1</v>
-      </c>
-      <c r="BV2">
-        <v>1</v>
-      </c>
-      <c r="BW2">
-        <v>1</v>
-      </c>
-      <c r="BX2">
-        <v>1</v>
-      </c>
-      <c r="BY2">
-        <v>1</v>
-      </c>
-      <c r="BZ2">
-        <v>1</v>
-      </c>
-      <c r="CA2">
-        <v>1</v>
-      </c>
-      <c r="CB2">
-        <v>1</v>
-      </c>
-      <c r="CC2">
-        <v>1</v>
-      </c>
-      <c r="CD2">
-        <v>1</v>
-      </c>
-      <c r="CE2">
-        <v>1</v>
-      </c>
-      <c r="CF2">
-        <v>1</v>
-      </c>
-      <c r="CG2">
-        <v>1</v>
-      </c>
-      <c r="CH2">
-        <v>0</v>
-      </c>
-      <c r="CI2">
-        <v>0</v>
-      </c>
-      <c r="CJ2">
-        <v>0</v>
-      </c>
-      <c r="CK2">
-        <v>0</v>
-      </c>
-      <c r="CL2">
-        <v>0</v>
-      </c>
-      <c r="CM2">
-        <v>0</v>
-      </c>
-      <c r="CN2">
-        <v>0</v>
-      </c>
-      <c r="CO2">
-        <v>0</v>
-      </c>
-      <c r="CP2">
-        <v>0</v>
-      </c>
-      <c r="CQ2">
-        <v>0</v>
-      </c>
-      <c r="CR2">
-        <v>0</v>
-      </c>
-      <c r="CS2">
-        <v>0</v>
-      </c>
-      <c r="CT2">
-        <v>0</v>
-      </c>
-      <c r="CU2">
-        <v>0</v>
-      </c>
-      <c r="CV2">
-        <v>0</v>
-      </c>
-      <c r="CW2">
-        <v>0</v>
-      </c>
-      <c r="CX2">
-        <v>0</v>
-      </c>
-      <c r="CY2">
-        <v>0</v>
-      </c>
-      <c r="CZ2">
-        <v>0</v>
-      </c>
-      <c r="DA2">
-        <v>0</v>
-      </c>
-      <c r="DB2">
-        <v>0</v>
-      </c>
-      <c r="DC2">
-        <v>0</v>
-      </c>
-      <c r="DD2">
-        <v>0</v>
-      </c>
-      <c r="DE2">
-        <v>0</v>
-      </c>
-      <c r="DF2">
-        <v>0</v>
-      </c>
-      <c r="DG2">
-        <v>0</v>
-      </c>
-      <c r="DH2">
-        <v>0</v>
-      </c>
-      <c r="DI2">
-        <v>0</v>
-      </c>
-      <c r="DJ2">
-        <v>0</v>
-      </c>
-      <c r="DK2">
-        <v>0</v>
-      </c>
-      <c r="DL2">
-        <v>0</v>
-      </c>
-      <c r="DM2">
-        <v>0</v>
-      </c>
-      <c r="DN2">
-        <v>0</v>
-      </c>
-      <c r="DO2">
-        <v>0</v>
-      </c>
-      <c r="DP2">
-        <v>0</v>
-      </c>
-      <c r="DQ2">
-        <v>0</v>
-      </c>
-      <c r="DR2">
-        <v>0</v>
-      </c>
-      <c r="DS2">
-        <v>0</v>
-      </c>
-      <c r="DT2">
-        <v>0</v>
-      </c>
-      <c r="DU2">
-        <v>0</v>
-      </c>
-      <c r="DV2">
-        <v>0</v>
-      </c>
-      <c r="DW2">
-        <v>0</v>
-      </c>
-      <c r="DX2">
-        <v>0</v>
-      </c>
-      <c r="DY2">
-        <v>0</v>
-      </c>
-      <c r="DZ2">
-        <v>0</v>
-      </c>
-      <c r="EA2">
-        <v>0</v>
-      </c>
-      <c r="EB2">
-        <v>0</v>
-      </c>
-      <c r="EC2">
-        <v>0</v>
-      </c>
-      <c r="ED2">
-        <v>0</v>
-      </c>
-      <c r="EE2">
-        <v>0</v>
-      </c>
-      <c r="EF2">
-        <v>0</v>
-      </c>
-      <c r="EG2">
-        <v>0</v>
-      </c>
-      <c r="EH2">
-        <v>0</v>
-      </c>
-      <c r="EI2">
-        <v>0</v>
-      </c>
-      <c r="EJ2">
-        <v>0</v>
-      </c>
-      <c r="EK2">
-        <v>0</v>
-      </c>
-      <c r="EL2">
-        <v>0</v>
-      </c>
-      <c r="EM2">
-        <v>0</v>
-      </c>
-      <c r="EN2">
-        <v>0</v>
-      </c>
-      <c r="EO2">
-        <v>0</v>
-      </c>
-      <c r="EP2">
-        <v>0</v>
-      </c>
-      <c r="EQ2">
-        <v>0</v>
-      </c>
-      <c r="ER2">
-        <v>0</v>
-      </c>
-      <c r="ES2">
-        <v>0</v>
-      </c>
-      <c r="ET2">
-        <v>0</v>
-      </c>
-      <c r="EU2">
-        <v>0</v>
-      </c>
-      <c r="EV2">
-        <v>0</v>
-      </c>
-      <c r="EW2">
-        <v>0</v>
-      </c>
-      <c r="EX2">
-        <v>0</v>
-      </c>
-      <c r="EY2">
-        <v>0</v>
-      </c>
-      <c r="EZ2">
-        <v>0</v>
-      </c>
-      <c r="FA2">
-        <v>0</v>
-      </c>
-      <c r="FB2">
-        <v>0</v>
-      </c>
-      <c r="FC2">
-        <v>0</v>
-      </c>
-      <c r="FD2">
-        <v>0</v>
-      </c>
-      <c r="FE2">
-        <v>0</v>
-      </c>
-      <c r="FF2">
-        <v>0</v>
-      </c>
-      <c r="FG2">
-        <v>0</v>
-      </c>
-      <c r="FH2">
-        <v>0</v>
-      </c>
-      <c r="FI2">
-        <v>0</v>
-      </c>
-      <c r="FJ2">
-        <v>0</v>
-      </c>
-      <c r="FK2">
-        <v>0</v>
-      </c>
-      <c r="FL2">
-        <v>0</v>
-      </c>
-      <c r="FM2">
-        <v>0</v>
-      </c>
-      <c r="FN2">
-        <v>0</v>
-      </c>
-      <c r="FO2">
+      <c r="B2" s="2">
+        <v>1</v>
+      </c>
+      <c r="C2" s="2">
+        <v>1</v>
+      </c>
+      <c r="D2" s="2">
+        <v>1</v>
+      </c>
+      <c r="E2" s="2">
+        <v>1</v>
+      </c>
+      <c r="F2" s="2">
+        <v>1</v>
+      </c>
+      <c r="G2" s="2">
+        <v>1</v>
+      </c>
+      <c r="H2" s="2">
+        <v>1</v>
+      </c>
+      <c r="I2" s="2">
+        <v>1</v>
+      </c>
+      <c r="J2" s="2">
+        <v>1</v>
+      </c>
+      <c r="K2" s="2">
+        <v>1</v>
+      </c>
+      <c r="L2" s="2">
+        <v>1</v>
+      </c>
+      <c r="M2" s="2">
+        <v>1</v>
+      </c>
+      <c r="N2" s="2">
+        <v>1</v>
+      </c>
+      <c r="O2" s="2">
+        <v>1</v>
+      </c>
+      <c r="P2" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q2" s="2">
+        <v>1</v>
+      </c>
+      <c r="R2" s="2">
+        <v>1</v>
+      </c>
+      <c r="S2" s="2">
+        <v>1</v>
+      </c>
+      <c r="T2" s="2">
+        <v>1</v>
+      </c>
+      <c r="U2" s="2">
+        <v>1</v>
+      </c>
+      <c r="V2" s="2">
+        <v>1</v>
+      </c>
+      <c r="W2" s="2">
+        <v>1</v>
+      </c>
+      <c r="X2" s="2">
+        <v>1</v>
+      </c>
+      <c r="Y2" s="2">
+        <v>1</v>
+      </c>
+      <c r="Z2" s="2">
+        <v>1</v>
+      </c>
+      <c r="AA2" s="2">
+        <v>1</v>
+      </c>
+      <c r="AB2" s="2">
+        <v>1</v>
+      </c>
+      <c r="AC2" s="2">
+        <v>1</v>
+      </c>
+      <c r="AD2" s="2">
+        <v>1</v>
+      </c>
+      <c r="AE2" s="2">
+        <v>1</v>
+      </c>
+      <c r="AF2" s="2">
+        <v>1</v>
+      </c>
+      <c r="AG2" s="2">
+        <v>1</v>
+      </c>
+      <c r="AH2" s="2">
+        <v>1</v>
+      </c>
+      <c r="AI2" s="2">
+        <v>1</v>
+      </c>
+      <c r="AJ2" s="2">
+        <v>1</v>
+      </c>
+      <c r="AK2" s="2">
+        <v>1</v>
+      </c>
+      <c r="AL2" s="2">
+        <v>1</v>
+      </c>
+      <c r="AM2" s="2">
+        <v>1</v>
+      </c>
+      <c r="AN2" s="2">
+        <v>1</v>
+      </c>
+      <c r="AO2" s="2">
+        <v>1</v>
+      </c>
+      <c r="AP2" s="2">
+        <v>1</v>
+      </c>
+      <c r="AQ2" s="2">
+        <v>1</v>
+      </c>
+      <c r="AR2" s="2">
+        <v>1</v>
+      </c>
+      <c r="AS2" s="2">
+        <v>1</v>
+      </c>
+      <c r="AT2" s="2">
+        <v>1</v>
+      </c>
+      <c r="AU2" s="2">
+        <v>1</v>
+      </c>
+      <c r="AV2" s="2">
+        <v>1</v>
+      </c>
+      <c r="AW2" s="2">
+        <v>1</v>
+      </c>
+      <c r="AX2" s="2">
+        <v>1</v>
+      </c>
+      <c r="AY2" s="2">
+        <v>1</v>
+      </c>
+      <c r="AZ2" s="2">
+        <v>1</v>
+      </c>
+      <c r="BA2" s="2">
+        <v>1</v>
+      </c>
+      <c r="BB2" s="2">
+        <v>1</v>
+      </c>
+      <c r="BC2" s="2">
+        <v>1</v>
+      </c>
+      <c r="BD2" s="2">
+        <v>1</v>
+      </c>
+      <c r="BE2" s="2">
+        <v>1</v>
+      </c>
+      <c r="BF2" s="2">
+        <v>1</v>
+      </c>
+      <c r="BG2" s="2">
+        <v>1</v>
+      </c>
+      <c r="BH2" s="2">
+        <v>1</v>
+      </c>
+      <c r="BI2" s="2">
+        <v>1</v>
+      </c>
+      <c r="BJ2" s="2">
+        <v>1</v>
+      </c>
+      <c r="BK2" s="2">
+        <v>1</v>
+      </c>
+      <c r="BL2" s="2">
+        <v>1</v>
+      </c>
+      <c r="BM2" s="2">
+        <v>1</v>
+      </c>
+      <c r="BN2" s="2">
+        <v>1</v>
+      </c>
+      <c r="BO2" s="2">
+        <v>1</v>
+      </c>
+      <c r="BP2" s="2">
+        <v>1</v>
+      </c>
+      <c r="BQ2" s="2">
+        <v>1</v>
+      </c>
+      <c r="BR2" s="2">
+        <v>1</v>
+      </c>
+      <c r="BS2" s="2">
+        <v>1</v>
+      </c>
+      <c r="BT2" s="2">
+        <v>1</v>
+      </c>
+      <c r="BU2" s="2">
+        <v>1</v>
+      </c>
+      <c r="BV2" s="2">
+        <v>1</v>
+      </c>
+      <c r="BW2" s="2">
+        <v>1</v>
+      </c>
+      <c r="BX2" s="2">
+        <v>1</v>
+      </c>
+      <c r="BY2" s="2">
+        <v>1</v>
+      </c>
+      <c r="BZ2" s="2">
+        <v>1</v>
+      </c>
+      <c r="CA2" s="2">
+        <v>1</v>
+      </c>
+      <c r="CB2" s="2">
+        <v>1</v>
+      </c>
+      <c r="CC2" s="2">
+        <v>1</v>
+      </c>
+      <c r="CD2" s="2">
+        <v>1</v>
+      </c>
+      <c r="CE2" s="2">
+        <v>1</v>
+      </c>
+      <c r="CF2" s="2">
+        <v>1</v>
+      </c>
+      <c r="CG2" s="2">
+        <v>1</v>
+      </c>
+      <c r="CH2" s="2">
+        <v>0</v>
+      </c>
+      <c r="CI2" s="2">
+        <v>0</v>
+      </c>
+      <c r="CJ2" s="2">
+        <v>0</v>
+      </c>
+      <c r="CK2" s="2">
+        <v>0</v>
+      </c>
+      <c r="CL2" s="2">
+        <v>0</v>
+      </c>
+      <c r="CM2" s="2">
+        <v>0</v>
+      </c>
+      <c r="CN2" s="2">
+        <v>0</v>
+      </c>
+      <c r="CO2" s="2">
+        <v>0</v>
+      </c>
+      <c r="CP2" s="2">
+        <v>0</v>
+      </c>
+      <c r="CQ2" s="2">
+        <v>0</v>
+      </c>
+      <c r="CR2" s="2">
+        <v>0</v>
+      </c>
+      <c r="CS2" s="2">
+        <v>0</v>
+      </c>
+      <c r="CT2" s="2">
+        <v>0</v>
+      </c>
+      <c r="CU2" s="2">
+        <v>0</v>
+      </c>
+      <c r="CV2" s="2">
+        <v>0</v>
+      </c>
+      <c r="CW2" s="2">
+        <v>0</v>
+      </c>
+      <c r="CX2" s="2">
+        <v>0</v>
+      </c>
+      <c r="CY2" s="2">
+        <v>0</v>
+      </c>
+      <c r="CZ2" s="2">
+        <v>0</v>
+      </c>
+      <c r="DA2" s="2">
+        <v>0</v>
+      </c>
+      <c r="DB2" s="2">
+        <v>0</v>
+      </c>
+      <c r="DC2" s="2">
+        <v>0</v>
+      </c>
+      <c r="DD2" s="2">
+        <v>0</v>
+      </c>
+      <c r="DE2" s="2">
+        <v>0</v>
+      </c>
+      <c r="DF2" s="2">
+        <v>0</v>
+      </c>
+      <c r="DG2" s="2">
+        <v>0</v>
+      </c>
+      <c r="DH2" s="2">
+        <v>0</v>
+      </c>
+      <c r="DI2" s="2">
+        <v>0</v>
+      </c>
+      <c r="DJ2" s="2">
+        <v>0</v>
+      </c>
+      <c r="DK2" s="2">
+        <v>0</v>
+      </c>
+      <c r="DL2" s="2">
+        <v>0</v>
+      </c>
+      <c r="DM2" s="2">
+        <v>0</v>
+      </c>
+      <c r="DN2" s="2">
+        <v>0</v>
+      </c>
+      <c r="DO2" s="2">
+        <v>0</v>
+      </c>
+      <c r="DP2" s="2">
+        <v>0</v>
+      </c>
+      <c r="DQ2" s="2">
+        <v>0</v>
+      </c>
+      <c r="DR2" s="2">
+        <v>0</v>
+      </c>
+      <c r="DS2" s="2">
+        <v>0</v>
+      </c>
+      <c r="DT2" s="2">
+        <v>0</v>
+      </c>
+      <c r="DU2" s="2">
+        <v>0</v>
+      </c>
+      <c r="DV2" s="2">
+        <v>0</v>
+      </c>
+      <c r="DW2" s="2">
+        <v>0</v>
+      </c>
+      <c r="DX2" s="2">
+        <v>0</v>
+      </c>
+      <c r="DY2" s="2">
+        <v>0</v>
+      </c>
+      <c r="DZ2" s="2">
+        <v>0</v>
+      </c>
+      <c r="EA2" s="2">
+        <v>0</v>
+      </c>
+      <c r="EB2" s="2">
+        <v>0</v>
+      </c>
+      <c r="EC2" s="2">
+        <v>0</v>
+      </c>
+      <c r="ED2" s="2">
+        <v>0</v>
+      </c>
+      <c r="EE2" s="2">
+        <v>0</v>
+      </c>
+      <c r="EF2" s="2">
+        <v>0</v>
+      </c>
+      <c r="EG2" s="2">
+        <v>0</v>
+      </c>
+      <c r="EH2" s="2">
+        <v>0</v>
+      </c>
+      <c r="EI2" s="2">
+        <v>0</v>
+      </c>
+      <c r="EJ2" s="2">
+        <v>0</v>
+      </c>
+      <c r="EK2" s="2">
+        <v>0</v>
+      </c>
+      <c r="EL2" s="2">
+        <v>0</v>
+      </c>
+      <c r="EM2" s="2">
+        <v>0</v>
+      </c>
+      <c r="EN2" s="2">
+        <v>0</v>
+      </c>
+      <c r="EO2" s="2">
+        <v>0</v>
+      </c>
+      <c r="EP2" s="2">
+        <v>0</v>
+      </c>
+      <c r="EQ2" s="2">
+        <v>0</v>
+      </c>
+      <c r="ER2" s="2">
+        <v>0</v>
+      </c>
+      <c r="ES2" s="2">
+        <v>0</v>
+      </c>
+      <c r="ET2" s="2">
+        <v>0</v>
+      </c>
+      <c r="EU2" s="2">
+        <v>0</v>
+      </c>
+      <c r="EV2" s="2">
+        <v>0</v>
+      </c>
+      <c r="EW2" s="2">
+        <v>0</v>
+      </c>
+      <c r="EX2" s="2">
+        <v>0</v>
+      </c>
+      <c r="EY2" s="2">
+        <v>0</v>
+      </c>
+      <c r="EZ2" s="2">
+        <v>0</v>
+      </c>
+      <c r="FA2" s="2">
+        <v>0</v>
+      </c>
+      <c r="FB2" s="2">
+        <v>0</v>
+      </c>
+      <c r="FC2" s="2">
+        <v>0</v>
+      </c>
+      <c r="FD2" s="2">
+        <v>0</v>
+      </c>
+      <c r="FE2" s="2">
+        <v>0</v>
+      </c>
+      <c r="FF2" s="2">
+        <v>0</v>
+      </c>
+      <c r="FG2" s="2">
+        <v>0</v>
+      </c>
+      <c r="FH2" s="2">
+        <v>0</v>
+      </c>
+      <c r="FI2" s="2">
+        <v>0</v>
+      </c>
+      <c r="FJ2" s="2">
+        <v>0</v>
+      </c>
+      <c r="FK2" s="2">
+        <v>0</v>
+      </c>
+      <c r="FL2" s="2">
+        <v>0</v>
+      </c>
+      <c r="FM2" s="2">
+        <v>0</v>
+      </c>
+      <c r="FN2" s="2">
+        <v>0</v>
+      </c>
+      <c r="FO2" s="2">
+        <v>0</v>
+      </c>
+      <c r="FP2" s="2">
+        <v>1</v>
+      </c>
+      <c r="FQ2" s="2">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:173" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:178" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -2152,14 +2225,20 @@
       <c r="FO3">
         <v>0</v>
       </c>
-      <c r="FP3" t="s">
+      <c r="FP3">
+        <v>0</v>
+      </c>
+      <c r="FQ3">
+        <v>3</v>
+      </c>
+      <c r="FU3" t="s">
         <v>57</v>
       </c>
-      <c r="FQ3" t="s">
+      <c r="FV3" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="4" spans="1:173" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:178" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -2673,14 +2752,20 @@
       <c r="FO4">
         <v>0</v>
       </c>
-      <c r="FP4" t="s">
+      <c r="FP4">
+        <v>0</v>
+      </c>
+      <c r="FQ4">
+        <v>3</v>
+      </c>
+      <c r="FU4" t="s">
         <v>57</v>
       </c>
-      <c r="FQ4" t="s">
+      <c r="FV4" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="5" spans="1:173" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:178" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -3194,14 +3279,20 @@
       <c r="FO5">
         <v>0</v>
       </c>
-      <c r="FP5" t="s">
+      <c r="FP5">
+        <v>1</v>
+      </c>
+      <c r="FQ5">
+        <v>3</v>
+      </c>
+      <c r="FU5" t="s">
         <v>57</v>
       </c>
-      <c r="FQ5" t="s">
+      <c r="FV5" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="6" spans="1:173" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:178" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -3715,14 +3806,20 @@
       <c r="FO6">
         <v>0</v>
       </c>
-      <c r="FP6" t="s">
+      <c r="FP6">
+        <v>2</v>
+      </c>
+      <c r="FQ6">
+        <v>2</v>
+      </c>
+      <c r="FU6" t="s">
         <v>57</v>
       </c>
-      <c r="FQ6" t="s">
+      <c r="FV6" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="7" spans="1:173" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:178" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -4236,14 +4333,20 @@
       <c r="FO7">
         <v>0</v>
       </c>
-      <c r="FP7" t="s">
+      <c r="FP7">
+        <v>3</v>
+      </c>
+      <c r="FQ7">
+        <v>3</v>
+      </c>
+      <c r="FU7" t="s">
         <v>57</v>
       </c>
-      <c r="FQ7" t="s">
+      <c r="FV7" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="8" spans="1:173" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:178" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -4757,14 +4860,20 @@
       <c r="FO8">
         <v>0</v>
       </c>
-      <c r="FP8" t="s">
+      <c r="FP8">
+        <v>1</v>
+      </c>
+      <c r="FQ8">
+        <v>1</v>
+      </c>
+      <c r="FU8" t="s">
         <v>58</v>
       </c>
-      <c r="FQ8" t="s">
+      <c r="FV8" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="9" spans="1:173" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:178" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -5278,14 +5387,20 @@
       <c r="FO9">
         <v>0</v>
       </c>
-      <c r="FP9" t="s">
+      <c r="FP9">
+        <v>1</v>
+      </c>
+      <c r="FQ9">
+        <v>1</v>
+      </c>
+      <c r="FU9" t="s">
         <v>58</v>
       </c>
-      <c r="FQ9" t="s">
+      <c r="FV9" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="10" spans="1:173" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:178" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -5799,14 +5914,20 @@
       <c r="FO10">
         <v>1</v>
       </c>
-      <c r="FP10" t="s">
+      <c r="FP10">
+        <v>3</v>
+      </c>
+      <c r="FQ10">
+        <v>3</v>
+      </c>
+      <c r="FU10" t="s">
         <v>57</v>
       </c>
-      <c r="FQ10" t="s">
+      <c r="FV10" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="11" spans="1:173" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:178" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -6320,14 +6441,20 @@
       <c r="FO11">
         <v>0</v>
       </c>
-      <c r="FP11" t="s">
+      <c r="FP11">
+        <v>3</v>
+      </c>
+      <c r="FQ11">
+        <v>3</v>
+      </c>
+      <c r="FU11" t="s">
         <v>57</v>
       </c>
-      <c r="FQ11" t="s">
+      <c r="FV11" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="12" spans="1:173" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:178" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -6841,14 +6968,20 @@
       <c r="FO12">
         <v>0</v>
       </c>
-      <c r="FP12" t="s">
+      <c r="FP12">
+        <v>1</v>
+      </c>
+      <c r="FQ12">
+        <v>2</v>
+      </c>
+      <c r="FU12" t="s">
         <v>57</v>
       </c>
-      <c r="FQ12" t="s">
+      <c r="FV12" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="13" spans="1:173" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:178" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>11</v>
       </c>
@@ -7362,14 +7495,20 @@
       <c r="FO13">
         <v>0</v>
       </c>
-      <c r="FP13" t="s">
+      <c r="FP13">
+        <v>1</v>
+      </c>
+      <c r="FQ13">
+        <v>3</v>
+      </c>
+      <c r="FU13" t="s">
         <v>57</v>
       </c>
-      <c r="FQ13" t="s">
+      <c r="FV13" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="14" spans="1:173" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:178" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>12</v>
       </c>
@@ -7883,14 +8022,20 @@
       <c r="FO14">
         <v>1</v>
       </c>
-      <c r="FP14" t="s">
+      <c r="FP14">
+        <v>3</v>
+      </c>
+      <c r="FQ14">
+        <v>4</v>
+      </c>
+      <c r="FU14" t="s">
         <v>57</v>
       </c>
-      <c r="FQ14" t="s">
+      <c r="FV14" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="15" spans="1:173" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:178" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>13</v>
       </c>
@@ -8404,14 +8549,20 @@
       <c r="FO15">
         <v>1</v>
       </c>
-      <c r="FP15" t="s">
+      <c r="FP15">
+        <v>3</v>
+      </c>
+      <c r="FQ15">
+        <v>3</v>
+      </c>
+      <c r="FU15" t="s">
         <v>57</v>
       </c>
-      <c r="FQ15" t="s">
+      <c r="FV15" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="16" spans="1:173" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:178" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>14</v>
       </c>
@@ -8925,14 +9076,20 @@
       <c r="FO16">
         <v>1</v>
       </c>
-      <c r="FP16" t="s">
+      <c r="FP16">
+        <v>2</v>
+      </c>
+      <c r="FQ16">
+        <v>2</v>
+      </c>
+      <c r="FU16" t="s">
         <v>57</v>
       </c>
-      <c r="FQ16" t="s">
+      <c r="FV16" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="17" spans="1:173" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:178" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>15</v>
       </c>
@@ -9446,14 +9603,20 @@
       <c r="FO17">
         <v>0</v>
       </c>
-      <c r="FP17" t="s">
+      <c r="FP17">
+        <v>2</v>
+      </c>
+      <c r="FQ17">
+        <v>3</v>
+      </c>
+      <c r="FU17" t="s">
         <v>57</v>
       </c>
-      <c r="FQ17" t="s">
+      <c r="FV17" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="18" spans="1:173" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:178" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>16</v>
       </c>
@@ -9967,14 +10130,20 @@
       <c r="FO18">
         <v>0</v>
       </c>
-      <c r="FP18" t="s">
+      <c r="FP18">
+        <v>3</v>
+      </c>
+      <c r="FQ18">
+        <v>3</v>
+      </c>
+      <c r="FU18" t="s">
         <v>57</v>
       </c>
-      <c r="FQ18" t="s">
+      <c r="FV18" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="19" spans="1:173" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:178" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>17</v>
       </c>
@@ -10488,14 +10657,20 @@
       <c r="FO19">
         <v>0</v>
       </c>
-      <c r="FP19" t="s">
+      <c r="FP19">
+        <v>2</v>
+      </c>
+      <c r="FQ19">
+        <v>3</v>
+      </c>
+      <c r="FU19" t="s">
         <v>57</v>
       </c>
-      <c r="FQ19" t="s">
+      <c r="FV19" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="20" spans="1:173" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:178" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>18</v>
       </c>
@@ -11009,14 +11184,20 @@
       <c r="FO20">
         <v>0</v>
       </c>
-      <c r="FP20" t="s">
+      <c r="FP20">
+        <v>2</v>
+      </c>
+      <c r="FQ20">
+        <v>2</v>
+      </c>
+      <c r="FU20" t="s">
         <v>57</v>
       </c>
-      <c r="FQ20" t="s">
+      <c r="FV20" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="21" spans="1:173" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:178" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>19</v>
       </c>
@@ -11530,14 +11711,20 @@
       <c r="FO21">
         <v>0</v>
       </c>
-      <c r="FP21" t="s">
+      <c r="FP21">
+        <v>2</v>
+      </c>
+      <c r="FQ21">
+        <v>4</v>
+      </c>
+      <c r="FU21" t="s">
         <v>57</v>
       </c>
-      <c r="FQ21" t="s">
+      <c r="FV21" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="22" spans="1:173" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:178" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>20</v>
       </c>
@@ -12051,14 +12238,20 @@
       <c r="FO22">
         <v>1</v>
       </c>
-      <c r="FP22" t="s">
+      <c r="FP22">
+        <v>1</v>
+      </c>
+      <c r="FQ22">
+        <v>4</v>
+      </c>
+      <c r="FU22" t="s">
         <v>57</v>
       </c>
-      <c r="FQ22" t="s">
+      <c r="FV22" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="23" spans="1:173" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:178" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>21</v>
       </c>
@@ -12572,14 +12765,20 @@
       <c r="FO23">
         <v>1</v>
       </c>
-      <c r="FP23" t="s">
+      <c r="FP23">
+        <v>2</v>
+      </c>
+      <c r="FQ23">
+        <v>3</v>
+      </c>
+      <c r="FU23" t="s">
         <v>57</v>
       </c>
-      <c r="FQ23" t="s">
+      <c r="FV23" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="24" spans="1:173" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:178" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>22</v>
       </c>
@@ -13093,14 +13292,20 @@
       <c r="FO24">
         <v>0</v>
       </c>
-      <c r="FP24" t="s">
+      <c r="FP24">
+        <v>3</v>
+      </c>
+      <c r="FQ24">
+        <v>3</v>
+      </c>
+      <c r="FU24" t="s">
         <v>57</v>
       </c>
-      <c r="FQ24" t="s">
+      <c r="FV24" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="25" spans="1:173" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:178" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>23</v>
       </c>
@@ -13614,14 +13819,20 @@
       <c r="FO25">
         <v>1</v>
       </c>
-      <c r="FP25" t="s">
+      <c r="FP25">
+        <v>3</v>
+      </c>
+      <c r="FQ25">
+        <v>3</v>
+      </c>
+      <c r="FU25" t="s">
         <v>57</v>
       </c>
-      <c r="FQ25" t="s">
+      <c r="FV25" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="26" spans="1:173" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:178" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>24</v>
       </c>
@@ -14135,14 +14346,20 @@
       <c r="FO26">
         <v>1</v>
       </c>
-      <c r="FP26" t="s">
+      <c r="FP26">
+        <v>2</v>
+      </c>
+      <c r="FQ26">
+        <v>3</v>
+      </c>
+      <c r="FU26" t="s">
         <v>57</v>
       </c>
-      <c r="FQ26" t="s">
+      <c r="FV26" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="27" spans="1:173" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:178" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>25</v>
       </c>
@@ -14656,14 +14873,20 @@
       <c r="FO27">
         <v>0</v>
       </c>
-      <c r="FP27" t="s">
+      <c r="FP27">
+        <v>1</v>
+      </c>
+      <c r="FQ27">
+        <v>3</v>
+      </c>
+      <c r="FU27" t="s">
         <v>57</v>
       </c>
-      <c r="FQ27" t="s">
+      <c r="FV27" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="28" spans="1:173" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:178" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>26</v>
       </c>
@@ -15177,14 +15400,20 @@
       <c r="FO28">
         <v>0</v>
       </c>
-      <c r="FP28" t="s">
+      <c r="FP28">
+        <v>1</v>
+      </c>
+      <c r="FQ28">
+        <v>3</v>
+      </c>
+      <c r="FU28" t="s">
         <v>57</v>
       </c>
-      <c r="FQ28" t="s">
+      <c r="FV28" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="29" spans="1:173" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:178" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>27</v>
       </c>
@@ -15698,14 +15927,20 @@
       <c r="FO29">
         <v>0</v>
       </c>
-      <c r="FP29" t="s">
+      <c r="FP29">
+        <v>1</v>
+      </c>
+      <c r="FQ29">
+        <v>3</v>
+      </c>
+      <c r="FU29" t="s">
         <v>57</v>
       </c>
-      <c r="FQ29" t="s">
+      <c r="FV29" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="30" spans="1:173" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:178" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>28</v>
       </c>
@@ -16219,14 +16454,20 @@
       <c r="FO30">
         <v>0</v>
       </c>
-      <c r="FP30" t="s">
+      <c r="FP30">
+        <v>1</v>
+      </c>
+      <c r="FQ30">
+        <v>3</v>
+      </c>
+      <c r="FU30" t="s">
         <v>57</v>
       </c>
-      <c r="FQ30" t="s">
+      <c r="FV30" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="31" spans="1:173" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:178" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>29</v>
       </c>
@@ -16740,14 +16981,20 @@
       <c r="FO31">
         <v>0</v>
       </c>
-      <c r="FP31" t="s">
+      <c r="FP31">
+        <v>1</v>
+      </c>
+      <c r="FQ31">
+        <v>3</v>
+      </c>
+      <c r="FU31" t="s">
         <v>57</v>
       </c>
-      <c r="FQ31" t="s">
+      <c r="FV31" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="32" spans="1:173" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:178" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>30</v>
       </c>
@@ -17261,14 +17508,20 @@
       <c r="FO32">
         <v>0</v>
       </c>
-      <c r="FP32" t="s">
+      <c r="FP32">
+        <v>1</v>
+      </c>
+      <c r="FQ32">
+        <v>2</v>
+      </c>
+      <c r="FU32" t="s">
         <v>57</v>
       </c>
-      <c r="FQ32" t="s">
+      <c r="FV32" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="33" spans="1:173" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:178" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>31</v>
       </c>
@@ -17782,14 +18035,20 @@
       <c r="FO33">
         <v>1</v>
       </c>
-      <c r="FP33" t="s">
+      <c r="FP33">
+        <v>3</v>
+      </c>
+      <c r="FQ33">
+        <v>2</v>
+      </c>
+      <c r="FU33" t="s">
         <v>58</v>
       </c>
-      <c r="FQ33" t="s">
+      <c r="FV33" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="34" spans="1:173" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:178" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>32</v>
       </c>
@@ -18303,14 +18562,20 @@
       <c r="FO34">
         <v>3</v>
       </c>
-      <c r="FP34" t="s">
+      <c r="FP34">
+        <v>3</v>
+      </c>
+      <c r="FQ34">
+        <v>3</v>
+      </c>
+      <c r="FU34" t="s">
         <v>58</v>
       </c>
-      <c r="FQ34" t="s">
+      <c r="FV34" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="35" spans="1:173" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:178" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>33</v>
       </c>
@@ -18824,14 +19089,20 @@
       <c r="FO35">
         <v>0</v>
       </c>
-      <c r="FP35" t="s">
+      <c r="FP35">
+        <v>3</v>
+      </c>
+      <c r="FQ35">
+        <v>2</v>
+      </c>
+      <c r="FU35" t="s">
         <v>58</v>
       </c>
-      <c r="FQ35" t="s">
+      <c r="FV35" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="36" spans="1:173" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:178" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>34</v>
       </c>
@@ -19345,14 +19616,20 @@
       <c r="FO36">
         <v>0</v>
       </c>
-      <c r="FP36" t="s">
+      <c r="FP36">
+        <v>3</v>
+      </c>
+      <c r="FQ36">
+        <v>1</v>
+      </c>
+      <c r="FU36" t="s">
         <v>58</v>
       </c>
-      <c r="FQ36" t="s">
+      <c r="FV36" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="37" spans="1:173" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:178" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>35</v>
       </c>
@@ -19866,14 +20143,20 @@
       <c r="FO37">
         <v>0</v>
       </c>
-      <c r="FP37" t="s">
+      <c r="FP37">
+        <v>3</v>
+      </c>
+      <c r="FQ37">
+        <v>1</v>
+      </c>
+      <c r="FU37" t="s">
         <v>58</v>
       </c>
-      <c r="FQ37" t="s">
+      <c r="FV37" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="38" spans="1:173" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:178" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>36</v>
       </c>
@@ -20387,14 +20670,20 @@
       <c r="FO38">
         <v>0</v>
       </c>
-      <c r="FP38" t="s">
+      <c r="FP38">
+        <v>1</v>
+      </c>
+      <c r="FQ38">
+        <v>1</v>
+      </c>
+      <c r="FU38" t="s">
         <v>58</v>
       </c>
-      <c r="FQ38" t="s">
+      <c r="FV38" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="39" spans="1:173" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:178" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>37</v>
       </c>
@@ -20908,14 +21197,20 @@
       <c r="FO39">
         <v>0</v>
       </c>
-      <c r="FP39" t="s">
+      <c r="FP39">
+        <v>3</v>
+      </c>
+      <c r="FQ39">
+        <v>1</v>
+      </c>
+      <c r="FU39" t="s">
         <v>58</v>
       </c>
-      <c r="FQ39" t="s">
+      <c r="FV39" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="40" spans="1:173" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:178" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>38</v>
       </c>
@@ -21429,14 +21724,20 @@
       <c r="FO40">
         <v>0</v>
       </c>
-      <c r="FP40" t="s">
+      <c r="FP40">
+        <v>2</v>
+      </c>
+      <c r="FQ40">
+        <v>2</v>
+      </c>
+      <c r="FU40" t="s">
         <v>58</v>
       </c>
-      <c r="FQ40" t="s">
+      <c r="FV40" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="41" spans="1:173" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:178" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>39</v>
       </c>
@@ -21950,14 +22251,20 @@
       <c r="FO41">
         <v>0</v>
       </c>
-      <c r="FP41" t="s">
+      <c r="FP41">
+        <v>2</v>
+      </c>
+      <c r="FQ41">
+        <v>1</v>
+      </c>
+      <c r="FU41" t="s">
         <v>58</v>
       </c>
-      <c r="FQ41" t="s">
+      <c r="FV41" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="42" spans="1:173" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:178" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>40</v>
       </c>
@@ -22471,14 +22778,20 @@
       <c r="FO42">
         <v>0</v>
       </c>
-      <c r="FP42" t="s">
+      <c r="FP42">
+        <v>1</v>
+      </c>
+      <c r="FQ42">
+        <v>2</v>
+      </c>
+      <c r="FU42" t="s">
         <v>58</v>
       </c>
-      <c r="FQ42" t="s">
+      <c r="FV42" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="43" spans="1:173" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:178" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>41</v>
       </c>
@@ -22992,14 +23305,20 @@
       <c r="FO43">
         <v>0</v>
       </c>
-      <c r="FP43" t="s">
+      <c r="FP43">
+        <v>2</v>
+      </c>
+      <c r="FQ43">
+        <v>0</v>
+      </c>
+      <c r="FU43" t="s">
         <v>58</v>
       </c>
-      <c r="FQ43" t="s">
+      <c r="FV43" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="44" spans="1:173" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:178" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>42</v>
       </c>
@@ -23513,14 +23832,20 @@
       <c r="FO44">
         <v>2</v>
       </c>
-      <c r="FP44" t="s">
+      <c r="FP44">
+        <v>0</v>
+      </c>
+      <c r="FQ44">
+        <v>1</v>
+      </c>
+      <c r="FU44" t="s">
         <v>58</v>
       </c>
-      <c r="FQ44" t="s">
+      <c r="FV44" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="45" spans="1:173" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:178" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>43</v>
       </c>
@@ -24034,14 +24359,20 @@
       <c r="FO45">
         <v>2</v>
       </c>
-      <c r="FP45" t="s">
+      <c r="FP45">
+        <v>0</v>
+      </c>
+      <c r="FQ45">
+        <v>0</v>
+      </c>
+      <c r="FU45" t="s">
         <v>58</v>
       </c>
-      <c r="FQ45" t="s">
+      <c r="FV45" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="46" spans="1:173" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:178" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>44</v>
       </c>
@@ -24555,14 +24886,20 @@
       <c r="FO46">
         <v>0</v>
       </c>
-      <c r="FP46" t="s">
+      <c r="FP46">
+        <v>1</v>
+      </c>
+      <c r="FQ46">
+        <v>1</v>
+      </c>
+      <c r="FU46" t="s">
         <v>58</v>
       </c>
-      <c r="FQ46" t="s">
+      <c r="FV46" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="47" spans="1:173" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:178" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>45</v>
       </c>
@@ -25076,14 +25413,20 @@
       <c r="FO47">
         <v>1</v>
       </c>
-      <c r="FP47" t="s">
+      <c r="FP47">
+        <v>0</v>
+      </c>
+      <c r="FQ47">
+        <v>0</v>
+      </c>
+      <c r="FU47" t="s">
         <v>58</v>
       </c>
-      <c r="FQ47" t="s">
+      <c r="FV47" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="48" spans="1:173" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:178" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>46</v>
       </c>
@@ -25597,14 +25940,20 @@
       <c r="FO48">
         <v>3</v>
       </c>
-      <c r="FP48" t="s">
+      <c r="FP48">
+        <v>0</v>
+      </c>
+      <c r="FQ48">
+        <v>0</v>
+      </c>
+      <c r="FU48" t="s">
         <v>58</v>
       </c>
-      <c r="FQ48" t="s">
+      <c r="FV48" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="49" spans="1:173" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:178" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>47</v>
       </c>
@@ -26118,14 +26467,20 @@
       <c r="FO49">
         <v>4</v>
       </c>
-      <c r="FP49" t="s">
+      <c r="FP49">
+        <v>0</v>
+      </c>
+      <c r="FQ49">
+        <v>0</v>
+      </c>
+      <c r="FU49" t="s">
         <v>58</v>
       </c>
-      <c r="FQ49" t="s">
+      <c r="FV49" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="50" spans="1:173" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:178" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>48</v>
       </c>
@@ -26639,14 +26994,20 @@
       <c r="FO50">
         <v>4</v>
       </c>
-      <c r="FP50" t="s">
+      <c r="FP50">
+        <v>4</v>
+      </c>
+      <c r="FQ50">
+        <v>2</v>
+      </c>
+      <c r="FU50" t="s">
         <v>58</v>
       </c>
-      <c r="FQ50" t="s">
+      <c r="FV50" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="51" spans="1:173" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:178" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>49</v>
       </c>
@@ -27160,14 +27521,20 @@
       <c r="FO51">
         <v>0</v>
       </c>
-      <c r="FP51" t="s">
+      <c r="FP51">
+        <v>2</v>
+      </c>
+      <c r="FQ51">
+        <v>1</v>
+      </c>
+      <c r="FU51" t="s">
         <v>58</v>
       </c>
-      <c r="FQ51" t="s">
+      <c r="FV51" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="52" spans="1:173" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:178" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>50</v>
       </c>
@@ -27681,14 +28048,20 @@
       <c r="FO52">
         <v>1</v>
       </c>
-      <c r="FP52" t="s">
+      <c r="FP52">
+        <v>2</v>
+      </c>
+      <c r="FQ52">
+        <v>2</v>
+      </c>
+      <c r="FU52" t="s">
         <v>58</v>
       </c>
-      <c r="FQ52" t="s">
+      <c r="FV52" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="53" spans="1:173" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:178" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>51</v>
       </c>
@@ -28202,14 +28575,20 @@
       <c r="FO53">
         <v>3</v>
       </c>
-      <c r="FP53" t="s">
+      <c r="FP53">
+        <v>4</v>
+      </c>
+      <c r="FQ53">
+        <v>2</v>
+      </c>
+      <c r="FU53" t="s">
         <v>58</v>
       </c>
-      <c r="FQ53" t="s">
+      <c r="FV53" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="54" spans="1:173" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:178" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>52</v>
       </c>
@@ -28723,14 +29102,20 @@
       <c r="FO54">
         <v>3</v>
       </c>
-      <c r="FP54" t="s">
+      <c r="FP54">
+        <v>3</v>
+      </c>
+      <c r="FQ54">
+        <v>1</v>
+      </c>
+      <c r="FU54" t="s">
         <v>58</v>
       </c>
-      <c r="FQ54" t="s">
+      <c r="FV54" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="55" spans="1:173" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:178" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>53</v>
       </c>
@@ -29244,14 +29629,20 @@
       <c r="FO55">
         <v>3</v>
       </c>
-      <c r="FP55" t="s">
+      <c r="FP55">
+        <v>3</v>
+      </c>
+      <c r="FQ55">
+        <v>1</v>
+      </c>
+      <c r="FU55" t="s">
         <v>58</v>
       </c>
-      <c r="FQ55" t="s">
+      <c r="FV55" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="56" spans="1:173" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:178" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>54</v>
       </c>
@@ -29765,15 +30156,22 @@
       <c r="FO56">
         <v>1</v>
       </c>
-      <c r="FP56" t="s">
+      <c r="FP56">
+        <v>3</v>
+      </c>
+      <c r="FQ56">
+        <v>1</v>
+      </c>
+      <c r="FU56" t="s">
         <v>58</v>
       </c>
-      <c r="FQ56" t="s">
+      <c r="FV56" t="s">
         <v>64</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>